<commit_message>
Ajout des poignées sur la glissière
</commit_message>
<xml_diff>
--- a/parametresDimensions.xlsx
+++ b/parametresDimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Centrale\S8\Maquette numérique\Puissance4Catia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA3177E-2A8A-4CC0-A9B5-B6528849A24C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26D48A5-AE50-4A28-9B59-FAD211B90860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0E7BA13A-2A3F-4F17-B56A-7DE297F352BF}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final version Bugs corrected
</commit_message>
<xml_diff>
--- a/parametresDimensions.xlsx
+++ b/parametresDimensions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Centrale\S8\Maquette numérique\Puissance4Catia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26D48A5-AE50-4A28-9B59-FAD211B90860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BCF680-D8DD-4385-8A5E-DD84A4470E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0E7BA13A-2A3F-4F17-B56A-7DE297F352BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>hauteur (mm)</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>nombre_trous_vertical</t>
-  </si>
-  <si>
-    <t>longueur_prolongement_cotes (mm)</t>
   </si>
   <si>
     <t>epaisseur_plastique_fin (mm)</t>
@@ -422,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1841C418-3629-44D7-81CD-CA282391A768}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +507,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -518,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,18 +523,11 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>